<commit_message>
Updated the link to download AWS Products
Updated the broken link that has allows partners to download AWS Products and Partner Solutions.
Correct link: https://partnercentral.awspartner.com/OpportunityBulkImportPage
</commit_message>
<xml_diff>
--- a/opportunity-samples/Opportunity-FieldsAndStandardValues-DiffWithPrevVersion-V14.3.xlsx
+++ b/opportunity-samples/Opportunity-FieldsAndStandardValues-DiffWithPrevVersion-V14.3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10414"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aksmenon/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE07265E-F170-474E-B592-B9458EEA99B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84350E9-DEEC-3147-A2D8-FB68395198DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -4278,12 +4278,6 @@
     <t xml:space="preserve">Enables the linkage of solutions or offerings to opportunities. Insert the Offering IDs associated with the solutions being evaluated for addressing the customer's business problem. When an Offering ID isn't accessible, input "Other" and provide details in the "otherSolutionOffered" field. Offering IDs can be found AWS Partner Central &gt; Build &gt; Offering &gt; Offering Detail Page. The ID's format follows S-1234567 pattern. </t>
   </si>
   <si>
-    <t xml:space="preserve">New Field that takes multiple values separated by comma.
-For example, "awsProducts" : ["Lambda", "AWSManagedServices" , "WorkLink"]
-For obtaining the complete list of AWS Products, visit Partner Central &gt; Sell &gt; Opportunity Management. Click on Bulk Actions &gt; Import Opportunities &gt; Start Import. Link: https://partnercentral-uat.awspartner.aws.dev/OpportunityBulkImportPage
-Under Products and Offerings, Click on the link "Your Products and Offerings can be viewed here. </t>
-  </si>
-  <si>
     <t>If partner does not send a value for this field, AWS defaults it to "Net New Business"
 For backward compatability:
 For partners using version 1.0 payload, the field will default to  "Net New Business".</t>
@@ -4687,6 +4681,12 @@
   </si>
   <si>
     <t>Finalized Deployment Need</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Field that takes multiple values separated by comma.
+For example, "awsProducts" : ["Lambda", "AWSManagedServices" , "WorkLink"]
+For obtaining the complete list of AWS Products, visit Partner Central &gt; Sell &gt; Opportunity Management. Click on Bulk Actions &gt; Import Opportunities &gt; Start Import. Link: https://partnercentral.awspartner.com/OpportunityBulkImportPage
+Under Products and Offerings, Click on the link "Your Products and Offerings can be viewed here. </t>
   </si>
 </sst>
 </file>
@@ -5650,7 +5650,7 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="31"/>
       <c r="B2" s="63" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="C2" s="64"/>
       <c r="D2" s="31"/>
@@ -5665,7 +5665,7 @@
       <c r="A4" s="31"/>
       <c r="B4" s="47"/>
       <c r="C4" s="39" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="D4" s="31"/>
     </row>
@@ -5673,7 +5673,7 @@
       <c r="A5" s="31"/>
       <c r="B5" s="32"/>
       <c r="C5" s="33" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="D5" s="31"/>
     </row>
@@ -5681,7 +5681,7 @@
       <c r="A6" s="31"/>
       <c r="B6" s="32"/>
       <c r="C6" s="33" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="D6" s="31"/>
     </row>
@@ -5689,7 +5689,7 @@
       <c r="A7" s="31"/>
       <c r="B7" s="32"/>
       <c r="C7" s="33" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="D7" s="31"/>
     </row>
@@ -5697,7 +5697,7 @@
       <c r="A8" s="31"/>
       <c r="B8" s="32"/>
       <c r="C8" s="33" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="D8" s="31"/>
     </row>
@@ -5711,7 +5711,7 @@
       <c r="A10" s="31"/>
       <c r="B10" s="32"/>
       <c r="C10" s="33" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D10" s="31"/>
     </row>
@@ -5727,7 +5727,7 @@
       <c r="A12" s="31"/>
       <c r="B12" s="32"/>
       <c r="C12" s="33" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="D12" s="31"/>
     </row>
@@ -5735,7 +5735,7 @@
       <c r="A13" s="31"/>
       <c r="B13" s="32"/>
       <c r="C13" s="33" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="D13" s="31"/>
     </row>
@@ -5743,7 +5743,7 @@
       <c r="A14" s="31"/>
       <c r="B14" s="32"/>
       <c r="C14" s="33" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="D14" s="31"/>
     </row>
@@ -5751,7 +5751,7 @@
       <c r="A15" s="31"/>
       <c r="B15" s="32"/>
       <c r="C15" s="33" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="D15" s="31"/>
     </row>
@@ -5759,7 +5759,7 @@
       <c r="A16" s="31"/>
       <c r="B16" s="32"/>
       <c r="C16" s="33" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="D16" s="31"/>
     </row>
@@ -5772,7 +5772,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="31"/>
       <c r="B18" s="65" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="C18" s="66"/>
       <c r="D18" s="31"/>
@@ -5821,7 +5821,7 @@
       <c r="A24" s="31"/>
       <c r="B24" s="32"/>
       <c r="C24" s="33" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="D24" s="31"/>
     </row>
@@ -5829,7 +5829,7 @@
       <c r="A25" s="31"/>
       <c r="B25" s="32"/>
       <c r="C25" s="33" t="s">
-        <v>1389</v>
+        <v>1388</v>
       </c>
       <c r="D25" s="31"/>
     </row>
@@ -5869,7 +5869,7 @@
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="33" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="D30" s="31"/>
     </row>
@@ -5885,14 +5885,14 @@
       <c r="A32" s="31"/>
       <c r="B32" s="32"/>
       <c r="C32" s="33" t="s">
-        <v>1388</v>
+        <v>1387</v>
       </c>
       <c r="D32" s="31"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="31"/>
       <c r="B33" s="65" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="C33" s="66"/>
       <c r="D33" s="31"/>
@@ -5901,7 +5901,7 @@
       <c r="A34" s="31"/>
       <c r="B34" s="47"/>
       <c r="C34" s="33" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="D34" s="31"/>
     </row>
@@ -5909,7 +5909,7 @@
       <c r="A35" s="31"/>
       <c r="B35" s="47"/>
       <c r="C35" s="33" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="D35" s="31"/>
     </row>
@@ -5957,9 +5957,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q102"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A48" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H73" sqref="H73"/>
+      <selection pane="topRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6007,16 +6007,16 @@
         <v>5</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>1395</v>
+        <v>1394</v>
       </c>
       <c r="J1" s="18" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="18" t="s">
+        <v>1395</v>
+      </c>
+      <c r="L1" s="18" t="s">
         <v>1396</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>1397</v>
       </c>
       <c r="M1" s="18" t="s">
         <v>7</v>
@@ -6151,7 +6151,7 @@
         <v>33</v>
       </c>
       <c r="H4" s="21" t="s">
-        <v>1390</v>
+        <v>1389</v>
       </c>
       <c r="I4" s="21" t="s">
         <v>34</v>
@@ -6608,7 +6608,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="238" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>84</v>
       </c>
@@ -6628,8 +6628,8 @@
       <c r="G14" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="H14" s="19" t="s">
-        <v>1385</v>
+      <c r="H14" s="20" t="s">
+        <v>1429</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>28</v>
@@ -6778,7 +6778,7 @@
         <v>104</v>
       </c>
       <c r="H17" s="43" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="I17" s="40" t="s">
         <v>34</v>
@@ -6971,7 +6971,7 @@
       </c>
       <c r="H21" s="36"/>
       <c r="I21" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="3" t="s">
@@ -7060,7 +7060,7 @@
         <v>132</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>1386</v>
+        <v>1385</v>
       </c>
       <c r="I23" s="19" t="s">
         <v>28</v>
@@ -7109,7 +7109,7 @@
         <v>137</v>
       </c>
       <c r="H24" s="19" t="s">
-        <v>1393</v>
+        <v>1392</v>
       </c>
       <c r="I24" s="19" t="s">
         <v>19</v>
@@ -7448,13 +7448,13 @@
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="19" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="G31" s="19" t="s">
         <v>1384</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="I31" s="19" t="s">
         <v>34</v>
@@ -7823,7 +7823,7 @@
       </c>
       <c r="H39" s="36"/>
       <c r="I39" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>35</v>
@@ -7870,7 +7870,7 @@
       </c>
       <c r="H40" s="36"/>
       <c r="I40" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>35</v>
@@ -7917,7 +7917,7 @@
       </c>
       <c r="H41" s="36"/>
       <c r="I41" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>35</v>
@@ -7926,7 +7926,7 @@
         <v>28</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="M41" s="3" t="s">
         <v>123</v>
@@ -7964,7 +7964,7 @@
       </c>
       <c r="H42" s="36"/>
       <c r="I42" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J42" s="3" t="s">
         <v>35</v>
@@ -7973,7 +7973,7 @@
         <v>28</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="M42" s="3" t="s">
         <v>123</v>
@@ -8011,7 +8011,7 @@
       </c>
       <c r="H43" s="36"/>
       <c r="I43" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J43" s="3" t="s">
         <v>35</v>
@@ -8058,7 +8058,7 @@
       </c>
       <c r="H44" s="36"/>
       <c r="I44" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>35</v>
@@ -8104,7 +8104,7 @@
         <v>240</v>
       </c>
       <c r="H45" s="44" t="s">
-        <v>1391</v>
+        <v>1390</v>
       </c>
       <c r="I45" s="40" t="s">
         <v>28</v>
@@ -8149,7 +8149,7 @@
         <v>244</v>
       </c>
       <c r="H46" s="44" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="I46" s="40" t="s">
         <v>28</v>
@@ -8194,7 +8194,7 @@
         <v>248</v>
       </c>
       <c r="H47" s="44" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="I47" s="40" t="s">
         <v>28</v>
@@ -8239,7 +8239,7 @@
         <v>253</v>
       </c>
       <c r="H48" s="44" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="I48" s="40" t="s">
         <v>28</v>
@@ -8284,7 +8284,7 @@
         <v>257</v>
       </c>
       <c r="H49" s="44" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="I49" s="40" t="s">
         <v>28</v>
@@ -8330,14 +8330,14 @@
       </c>
       <c r="H50" s="36"/>
       <c r="I50" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="M50" s="3" t="s">
         <v>123</v>
@@ -8375,14 +8375,14 @@
       </c>
       <c r="H51" s="36"/>
       <c r="I51" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="M51" s="3" t="s">
         <v>123</v>
@@ -8651,7 +8651,7 @@
       </c>
       <c r="H57" s="36"/>
       <c r="I57" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>35</v>
@@ -8660,7 +8660,7 @@
         <v>28</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="M57" s="3" t="s">
         <v>123</v>
@@ -8698,7 +8698,7 @@
       </c>
       <c r="H58" s="36"/>
       <c r="I58" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>35</v>
@@ -8707,7 +8707,7 @@
         <v>28</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="M58" s="3" t="s">
         <v>123</v>
@@ -8745,7 +8745,7 @@
       </c>
       <c r="H59" s="36"/>
       <c r="I59" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J59" s="3" t="s">
         <v>35</v>
@@ -8754,7 +8754,7 @@
         <v>28</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="M59" s="3" t="s">
         <v>123</v>
@@ -8792,7 +8792,7 @@
       </c>
       <c r="H60" s="36"/>
       <c r="I60" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>35</v>
@@ -8801,7 +8801,7 @@
         <v>28</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="M60" s="3" t="s">
         <v>123</v>
@@ -8888,7 +8888,7 @@
       </c>
       <c r="H62" s="36"/>
       <c r="I62" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J62" s="1"/>
       <c r="K62" s="3" t="s">
@@ -9031,7 +9031,7 @@
       </c>
       <c r="H65" s="19"/>
       <c r="I65" s="19" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J65" s="19"/>
       <c r="K65" s="19" t="s">
@@ -9074,7 +9074,7 @@
       </c>
       <c r="H66" s="19"/>
       <c r="I66" s="19" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J66" s="19"/>
       <c r="K66" s="19" t="s">
@@ -9128,7 +9128,7 @@
         <v>34</v>
       </c>
       <c r="L67" s="36" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="M67" s="3" t="s">
         <v>21</v>
@@ -9168,7 +9168,7 @@
       </c>
       <c r="H68" s="36"/>
       <c r="I68" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J68" s="3" t="s">
         <v>35</v>
@@ -9265,7 +9265,7 @@
         <v>19</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="K70" s="3" t="s">
         <v>28</v>
@@ -9275,7 +9275,7 @@
         <v>21</v>
       </c>
       <c r="N70" s="3" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="O70" s="3" t="s">
         <v>22</v>
@@ -9312,7 +9312,7 @@
         <v>19</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="K71" s="3" t="s">
         <v>28</v>
@@ -9322,7 +9322,7 @@
         <v>21</v>
       </c>
       <c r="N71" s="3" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="O71" s="3" t="s">
         <v>22</v>
@@ -9357,7 +9357,7 @@
         <v>19</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="K72" s="3" t="s">
         <v>28</v>
@@ -9367,7 +9367,7 @@
         <v>21</v>
       </c>
       <c r="N72" s="3" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="O72" s="3" t="s">
         <v>22</v>
@@ -9402,7 +9402,7 @@
         <v>19</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="K73" s="3" t="s">
         <v>28</v>
@@ -9412,7 +9412,7 @@
         <v>21</v>
       </c>
       <c r="N73" s="3" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="O73" s="3" t="s">
         <v>22</v>
@@ -9449,7 +9449,7 @@
         <v>19</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="K74" s="3" t="s">
         <v>28</v>
@@ -9459,7 +9459,7 @@
         <v>21</v>
       </c>
       <c r="N74" s="3" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="O74" s="3" t="s">
         <v>22</v>
@@ -9493,7 +9493,7 @@
       </c>
       <c r="H75" s="36"/>
       <c r="I75" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J75" s="1"/>
       <c r="K75" s="38" t="s">
@@ -9632,7 +9632,7 @@
       </c>
       <c r="H78" s="36"/>
       <c r="I78" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J78" s="1"/>
       <c r="K78" s="38" t="s">
@@ -9769,7 +9769,7 @@
       </c>
       <c r="H81" s="36"/>
       <c r="I81" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J81" s="3" t="s">
         <v>35</v>
@@ -9816,7 +9816,7 @@
       </c>
       <c r="H82" s="36"/>
       <c r="I82" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J82" s="3" t="s">
         <v>35</v>
@@ -9863,7 +9863,7 @@
       </c>
       <c r="H83" s="36"/>
       <c r="I83" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J83" s="3" t="s">
         <v>35</v>
@@ -9910,7 +9910,7 @@
       </c>
       <c r="H84" s="36"/>
       <c r="I84" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J84" s="3" t="s">
         <v>35</v>
@@ -9957,7 +9957,7 @@
       </c>
       <c r="H85" s="36"/>
       <c r="I85" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J85" s="3" t="s">
         <v>35</v>
@@ -10004,7 +10004,7 @@
       </c>
       <c r="H86" s="36"/>
       <c r="I86" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J86" s="1"/>
       <c r="K86" s="38" t="s">
@@ -10047,7 +10047,7 @@
       </c>
       <c r="H87" s="36"/>
       <c r="I87" s="3" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J87" s="1"/>
       <c r="K87" s="38" t="s">
@@ -10087,7 +10087,7 @@
         <v>415</v>
       </c>
       <c r="H88" s="21" t="s">
-        <v>1387</v>
+        <v>1386</v>
       </c>
       <c r="I88" s="21" t="s">
         <v>34</v>
@@ -10180,14 +10180,14 @@
         <v>138</v>
       </c>
       <c r="I90" s="19" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J90" s="19"/>
       <c r="K90" s="19" t="s">
         <v>19</v>
       </c>
       <c r="L90" s="19" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="M90" s="19" t="s">
         <v>123</v>
@@ -10223,14 +10223,14 @@
       </c>
       <c r="H91" s="19"/>
       <c r="I91" s="19" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="J91" s="19"/>
       <c r="K91" s="19" t="s">
         <v>19</v>
       </c>
       <c r="L91" s="19" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="M91" s="19" t="s">
         <v>123</v>
@@ -10811,7 +10811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD253"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -11480,7 +11480,7 @@
     </row>
     <row r="9" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -12108,7 +12108,7 @@
         <v>732</v>
       </c>
       <c r="O20" s="46" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="P20" s="13"/>
       <c r="Q20" s="13"/>

</xml_diff>

<commit_message>
Ported the changes on the CSV to the Excel
- Updated details of AWS Solution link
- More specifics on AWSX Products
- AWS Linking is required for OfferID linking
</commit_message>
<xml_diff>
--- a/opportunity-samples/Opportunity-FieldsAndStandardValues-DiffWithPrevVersion-V14.3.xlsx
+++ b/opportunity-samples/Opportunity-FieldsAndStandardValues-DiffWithPrevVersion-V14.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aksmenon/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84350E9-DEEC-3147-A2D8-FB68395198DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CE17B8-7911-0D46-89DA-04314B1E5E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4329,13 +4329,6 @@
     </r>
   </si>
   <si>
-    <t>To get a list of solutions in your Partner Central Account, visit Partner Central &gt; Sell &gt; Opportunity Management. Click on Bulk Actions &gt; Import Opportunities &gt; Start Import. Link: https://partnercentral-uat.awspartner.aws.dev/OpportunityBulkImportPage
-Under Products and Offerings, Click on the link "Your Products and Offerings can be viewed here. 
-When an AWS Originated Opportunity is shared, this field is masked and comes with a value null. This field is mandatory in the payload from Partner to AWS and but may be null in the payload from AWS to Partner.
-For backward compatability:
-For partners in old verison, the value will be deafulted to "Other"</t>
-  </si>
-  <si>
     <t>Inbound - Mandatory / Conditionally Mandatory / Optional</t>
   </si>
   <si>
@@ -4683,10 +4676,17 @@
     <t>Finalized Deployment Need</t>
   </si>
   <si>
-    <t xml:space="preserve">New Field that takes multiple values separated by comma.
+    <t>To get a list of solutions in your Partner Central Account, visit Partner Central &gt; Sell &gt; Opportunity Management. Click on Bulk Actions &gt; Import Opportunities &gt; Start Import. Link: https://partnercentral.awspartner.com/OpportunityBulkImportPage
+Use the solutionID values.
+When an AWS Originated Opportunity is shared, this field is masked and comes with a value null. This field is mandatory in the payload from Partner to AWS and but may be null in the payload from AWS to Partner.
+For backward compatability:
+For partners in old verison, the value will be deafulted to "Other"</t>
+  </si>
+  <si>
+    <t>New Field that takes multiple values separated by comma.
 For example, "awsProducts" : ["Lambda", "AWSManagedServices" , "WorkLink"]
 For obtaining the complete list of AWS Products, visit Partner Central &gt; Sell &gt; Opportunity Management. Click on Bulk Actions &gt; Import Opportunities &gt; Start Import. Link: https://partnercentral.awspartner.com/OpportunityBulkImportPage
-Under Products and Offerings, Click on the link "Your Products and Offerings can be viewed here. </t>
+Under Products and Offerings, Click on the link "Your Products and Offerings can be viewed here. Use the Product Codes and not the Product Names.</t>
   </si>
 </sst>
 </file>
@@ -5650,7 +5650,7 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="31"/>
       <c r="B2" s="63" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="C2" s="64"/>
       <c r="D2" s="31"/>
@@ -5665,7 +5665,7 @@
       <c r="A4" s="31"/>
       <c r="B4" s="47"/>
       <c r="C4" s="39" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="D4" s="31"/>
     </row>
@@ -5673,7 +5673,7 @@
       <c r="A5" s="31"/>
       <c r="B5" s="32"/>
       <c r="C5" s="33" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="D5" s="31"/>
     </row>
@@ -5681,7 +5681,7 @@
       <c r="A6" s="31"/>
       <c r="B6" s="32"/>
       <c r="C6" s="33" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="D6" s="31"/>
     </row>
@@ -5689,7 +5689,7 @@
       <c r="A7" s="31"/>
       <c r="B7" s="32"/>
       <c r="C7" s="33" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="D7" s="31"/>
     </row>
@@ -5697,7 +5697,7 @@
       <c r="A8" s="31"/>
       <c r="B8" s="32"/>
       <c r="C8" s="33" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="D8" s="31"/>
     </row>
@@ -5711,7 +5711,7 @@
       <c r="A10" s="31"/>
       <c r="B10" s="32"/>
       <c r="C10" s="33" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="D10" s="31"/>
     </row>
@@ -5727,7 +5727,7 @@
       <c r="A12" s="31"/>
       <c r="B12" s="32"/>
       <c r="C12" s="33" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="D12" s="31"/>
     </row>
@@ -5735,7 +5735,7 @@
       <c r="A13" s="31"/>
       <c r="B13" s="32"/>
       <c r="C13" s="33" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="D13" s="31"/>
     </row>
@@ -5743,7 +5743,7 @@
       <c r="A14" s="31"/>
       <c r="B14" s="32"/>
       <c r="C14" s="33" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="D14" s="31"/>
     </row>
@@ -5751,7 +5751,7 @@
       <c r="A15" s="31"/>
       <c r="B15" s="32"/>
       <c r="C15" s="33" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="D15" s="31"/>
     </row>
@@ -5759,7 +5759,7 @@
       <c r="A16" s="31"/>
       <c r="B16" s="32"/>
       <c r="C16" s="33" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="D16" s="31"/>
     </row>
@@ -5772,7 +5772,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="31"/>
       <c r="B18" s="65" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="C18" s="66"/>
       <c r="D18" s="31"/>
@@ -5821,7 +5821,7 @@
       <c r="A24" s="31"/>
       <c r="B24" s="32"/>
       <c r="C24" s="33" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="D24" s="31"/>
     </row>
@@ -5869,7 +5869,7 @@
       <c r="A30" s="31"/>
       <c r="B30" s="32"/>
       <c r="C30" s="33" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="D30" s="31"/>
     </row>
@@ -5892,7 +5892,7 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="31"/>
       <c r="B33" s="65" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="C33" s="66"/>
       <c r="D33" s="31"/>
@@ -5901,7 +5901,7 @@
       <c r="A34" s="31"/>
       <c r="B34" s="47"/>
       <c r="C34" s="33" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="D34" s="31"/>
     </row>
@@ -5909,7 +5909,7 @@
       <c r="A35" s="31"/>
       <c r="B35" s="47"/>
       <c r="C35" s="33" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="D35" s="31"/>
     </row>
@@ -5958,8 +5958,8 @@
   <dimension ref="A1:Q102"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H14" sqref="H14"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6007,16 +6007,16 @@
         <v>5</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>1394</v>
+        <v>1393</v>
       </c>
       <c r="J1" s="18" t="s">
         <v>6</v>
       </c>
       <c r="K1" s="18" t="s">
+        <v>1394</v>
+      </c>
+      <c r="L1" s="18" t="s">
         <v>1395</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>1396</v>
       </c>
       <c r="M1" s="18" t="s">
         <v>7</v>
@@ -6608,7 +6608,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="238" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" ht="255" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
         <v>84</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>104</v>
       </c>
       <c r="H17" s="43" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="I17" s="40" t="s">
         <v>34</v>
@@ -6971,7 +6971,7 @@
       </c>
       <c r="H21" s="36"/>
       <c r="I21" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="3" t="s">
@@ -7433,7 +7433,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:17" ht="255" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
         <v>176</v>
       </c>
@@ -7448,13 +7448,13 @@
       </c>
       <c r="E31" s="19"/>
       <c r="F31" s="19" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="G31" s="19" t="s">
         <v>1384</v>
       </c>
-      <c r="H31" s="19" t="s">
-        <v>1393</v>
+      <c r="H31" s="20" t="s">
+        <v>1428</v>
       </c>
       <c r="I31" s="19" t="s">
         <v>34</v>
@@ -7823,7 +7823,7 @@
       </c>
       <c r="H39" s="36"/>
       <c r="I39" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>35</v>
@@ -7870,7 +7870,7 @@
       </c>
       <c r="H40" s="36"/>
       <c r="I40" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J40" s="3" t="s">
         <v>35</v>
@@ -7917,7 +7917,7 @@
       </c>
       <c r="H41" s="36"/>
       <c r="I41" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>35</v>
@@ -7926,7 +7926,7 @@
         <v>28</v>
       </c>
       <c r="L41" s="3" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="M41" s="3" t="s">
         <v>123</v>
@@ -7964,7 +7964,7 @@
       </c>
       <c r="H42" s="36"/>
       <c r="I42" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J42" s="3" t="s">
         <v>35</v>
@@ -7973,7 +7973,7 @@
         <v>28</v>
       </c>
       <c r="L42" s="3" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="M42" s="3" t="s">
         <v>123</v>
@@ -8011,7 +8011,7 @@
       </c>
       <c r="H43" s="36"/>
       <c r="I43" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J43" s="3" t="s">
         <v>35</v>
@@ -8058,7 +8058,7 @@
       </c>
       <c r="H44" s="36"/>
       <c r="I44" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>35</v>
@@ -8330,14 +8330,14 @@
       </c>
       <c r="H50" s="36"/>
       <c r="I50" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L50" s="1" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="M50" s="3" t="s">
         <v>123</v>
@@ -8375,14 +8375,14 @@
       </c>
       <c r="H51" s="36"/>
       <c r="I51" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="3" t="s">
         <v>28</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="M51" s="3" t="s">
         <v>123</v>
@@ -8651,7 +8651,7 @@
       </c>
       <c r="H57" s="36"/>
       <c r="I57" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>35</v>
@@ -8660,7 +8660,7 @@
         <v>28</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="M57" s="3" t="s">
         <v>123</v>
@@ -8698,7 +8698,7 @@
       </c>
       <c r="H58" s="36"/>
       <c r="I58" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>35</v>
@@ -8707,7 +8707,7 @@
         <v>28</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="M58" s="3" t="s">
         <v>123</v>
@@ -8745,7 +8745,7 @@
       </c>
       <c r="H59" s="36"/>
       <c r="I59" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J59" s="3" t="s">
         <v>35</v>
@@ -8754,7 +8754,7 @@
         <v>28</v>
       </c>
       <c r="L59" s="3" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="M59" s="3" t="s">
         <v>123</v>
@@ -8792,7 +8792,7 @@
       </c>
       <c r="H60" s="36"/>
       <c r="I60" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J60" s="3" t="s">
         <v>35</v>
@@ -8801,7 +8801,7 @@
         <v>28</v>
       </c>
       <c r="L60" s="3" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="M60" s="3" t="s">
         <v>123</v>
@@ -8888,7 +8888,7 @@
       </c>
       <c r="H62" s="36"/>
       <c r="I62" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J62" s="1"/>
       <c r="K62" s="3" t="s">
@@ -9031,7 +9031,7 @@
       </c>
       <c r="H65" s="19"/>
       <c r="I65" s="19" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J65" s="19"/>
       <c r="K65" s="19" t="s">
@@ -9074,7 +9074,7 @@
       </c>
       <c r="H66" s="19"/>
       <c r="I66" s="19" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J66" s="19"/>
       <c r="K66" s="19" t="s">
@@ -9128,7 +9128,7 @@
         <v>34</v>
       </c>
       <c r="L67" s="36" t="s">
-        <v>1397</v>
+        <v>1396</v>
       </c>
       <c r="M67" s="3" t="s">
         <v>21</v>
@@ -9168,7 +9168,7 @@
       </c>
       <c r="H68" s="36"/>
       <c r="I68" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J68" s="3" t="s">
         <v>35</v>
@@ -9265,7 +9265,7 @@
         <v>19</v>
       </c>
       <c r="J70" s="3" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="K70" s="3" t="s">
         <v>28</v>
@@ -9275,7 +9275,7 @@
         <v>21</v>
       </c>
       <c r="N70" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="O70" s="3" t="s">
         <v>22</v>
@@ -9312,7 +9312,7 @@
         <v>19</v>
       </c>
       <c r="J71" s="3" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="K71" s="3" t="s">
         <v>28</v>
@@ -9322,7 +9322,7 @@
         <v>21</v>
       </c>
       <c r="N71" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="O71" s="3" t="s">
         <v>22</v>
@@ -9357,7 +9357,7 @@
         <v>19</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="K72" s="3" t="s">
         <v>28</v>
@@ -9367,7 +9367,7 @@
         <v>21</v>
       </c>
       <c r="N72" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="O72" s="3" t="s">
         <v>22</v>
@@ -9402,7 +9402,7 @@
         <v>19</v>
       </c>
       <c r="J73" s="3" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="K73" s="3" t="s">
         <v>28</v>
@@ -9412,7 +9412,7 @@
         <v>21</v>
       </c>
       <c r="N73" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="O73" s="3" t="s">
         <v>22</v>
@@ -9449,7 +9449,7 @@
         <v>19</v>
       </c>
       <c r="J74" s="3" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="K74" s="3" t="s">
         <v>28</v>
@@ -9459,7 +9459,7 @@
         <v>21</v>
       </c>
       <c r="N74" s="3" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="O74" s="3" t="s">
         <v>22</v>
@@ -9493,7 +9493,7 @@
       </c>
       <c r="H75" s="36"/>
       <c r="I75" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J75" s="1"/>
       <c r="K75" s="38" t="s">
@@ -9632,7 +9632,7 @@
       </c>
       <c r="H78" s="36"/>
       <c r="I78" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J78" s="1"/>
       <c r="K78" s="38" t="s">
@@ -9769,7 +9769,7 @@
       </c>
       <c r="H81" s="36"/>
       <c r="I81" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J81" s="3" t="s">
         <v>35</v>
@@ -9816,7 +9816,7 @@
       </c>
       <c r="H82" s="36"/>
       <c r="I82" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J82" s="3" t="s">
         <v>35</v>
@@ -9863,7 +9863,7 @@
       </c>
       <c r="H83" s="36"/>
       <c r="I83" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J83" s="3" t="s">
         <v>35</v>
@@ -9910,7 +9910,7 @@
       </c>
       <c r="H84" s="36"/>
       <c r="I84" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J84" s="3" t="s">
         <v>35</v>
@@ -9957,7 +9957,7 @@
       </c>
       <c r="H85" s="36"/>
       <c r="I85" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J85" s="3" t="s">
         <v>35</v>
@@ -10004,7 +10004,7 @@
       </c>
       <c r="H86" s="36"/>
       <c r="I86" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J86" s="1"/>
       <c r="K86" s="38" t="s">
@@ -10047,7 +10047,7 @@
       </c>
       <c r="H87" s="36"/>
       <c r="I87" s="3" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J87" s="1"/>
       <c r="K87" s="38" t="s">
@@ -10180,14 +10180,14 @@
         <v>138</v>
       </c>
       <c r="I90" s="19" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J90" s="19"/>
       <c r="K90" s="19" t="s">
         <v>19</v>
       </c>
       <c r="L90" s="19" t="s">
-        <v>1399</v>
+        <v>1398</v>
       </c>
       <c r="M90" s="19" t="s">
         <v>123</v>
@@ -10223,14 +10223,14 @@
       </c>
       <c r="H91" s="19"/>
       <c r="I91" s="19" t="s">
-        <v>1398</v>
+        <v>1397</v>
       </c>
       <c r="J91" s="19"/>
       <c r="K91" s="19" t="s">
         <v>19</v>
       </c>
       <c r="L91" s="19" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="M91" s="19" t="s">
         <v>123</v>
@@ -11480,7 +11480,7 @@
     </row>
     <row r="9" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -12108,7 +12108,7 @@
         <v>732</v>
       </c>
       <c r="O20" s="46" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="P20" s="13"/>
       <c r="Q20" s="13"/>

</xml_diff>